<commit_message>
Date: 05/17/2024 -> Update 2
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilshortland/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KyleWeldon\Projects\ThinkTank\S.P.A.R.T.A.N\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63ECD5F1-E8E5-E045-A0AE-920909463C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D400F0-9EB5-4DBE-927B-9B7B7A562537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3000" windowWidth="26040" windowHeight="13940" xr2:uid="{444940EF-C09F-FD4E-B664-1D711E050268}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7810" xr2:uid="{444940EF-C09F-FD4E-B664-1D711E050268}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -580,11 +580,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF53F7F-6300-0749-BD17-6E1343813F0F}">
   <dimension ref="A1:AX230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="7" width="10.83203125" style="2"/>
     <col min="8" max="13" width="10.83203125" style="3"/>
@@ -592,7 +592,7 @@
     <col min="18" max="28" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +744,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8648,7 +8648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9408,7 +9408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -10016,7 +10016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -10320,7 +10320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -10472,7 +10472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>66</v>
       </c>
@@ -10624,7 +10624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>68</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>69</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>70</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>71</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>72</v>
       </c>
@@ -11384,7 +11384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>73</v>
       </c>
@@ -11536,7 +11536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>74</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>75</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>76</v>
       </c>
@@ -11992,7 +11992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>77</v>
       </c>
@@ -12144,7 +12144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>78</v>
       </c>
@@ -12296,7 +12296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>79</v>
       </c>
@@ -12448,7 +12448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>80</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>81</v>
       </c>
@@ -12752,7 +12752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>82</v>
       </c>
@@ -12904,7 +12904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>83</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>84</v>
       </c>
@@ -13208,7 +13208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>85</v>
       </c>
@@ -13360,7 +13360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>86</v>
       </c>
@@ -13512,7 +13512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>87</v>
       </c>
@@ -13664,7 +13664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>88</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>89</v>
       </c>
@@ -13968,7 +13968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>90</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>91</v>
       </c>
@@ -14272,7 +14272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>92</v>
       </c>
@@ -14424,7 +14424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>93</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>94</v>
       </c>
@@ -14728,7 +14728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>95</v>
       </c>
@@ -14880,7 +14880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>96</v>
       </c>
@@ -15032,7 +15032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>97</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>98</v>
       </c>
@@ -15336,7 +15336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>99</v>
       </c>
@@ -15488,7 +15488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>100</v>
       </c>
@@ -15640,7 +15640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>101</v>
       </c>
@@ -15792,7 +15792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>102</v>
       </c>
@@ -15944,7 +15944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>103</v>
       </c>
@@ -16096,7 +16096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>104</v>
       </c>
@@ -16248,7 +16248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>105</v>
       </c>
@@ -16400,7 +16400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>106</v>
       </c>
@@ -16552,7 +16552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>107</v>
       </c>
@@ -16704,7 +16704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>108</v>
       </c>
@@ -16856,7 +16856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>109</v>
       </c>
@@ -17008,7 +17008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>110</v>
       </c>
@@ -17160,7 +17160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>111</v>
       </c>
@@ -17312,7 +17312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>112</v>
       </c>
@@ -17464,7 +17464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>113</v>
       </c>
@@ -17616,7 +17616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>114</v>
       </c>
@@ -17768,7 +17768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>115</v>
       </c>
@@ -17920,7 +17920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>116</v>
       </c>
@@ -18072,7 +18072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>117</v>
       </c>
@@ -18224,7 +18224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>118</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>119</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>120</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>121</v>
       </c>
@@ -18832,7 +18832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>122</v>
       </c>
@@ -18984,7 +18984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>123</v>
       </c>
@@ -19136,7 +19136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>124</v>
       </c>
@@ -19288,7 +19288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>125</v>
       </c>
@@ -19440,7 +19440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>126</v>
       </c>
@@ -19592,7 +19592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>127</v>
       </c>
@@ -19744,7 +19744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>128</v>
       </c>
@@ -19896,7 +19896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>129</v>
       </c>
@@ -20048,7 +20048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>130</v>
       </c>
@@ -20200,7 +20200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>131</v>
       </c>
@@ -20352,7 +20352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>132</v>
       </c>
@@ -20504,7 +20504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>133</v>
       </c>
@@ -20656,7 +20656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>134</v>
       </c>
@@ -20808,7 +20808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>135</v>
       </c>
@@ -20960,7 +20960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>136</v>
       </c>
@@ -21112,7 +21112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>137</v>
       </c>
@@ -21264,7 +21264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>138</v>
       </c>
@@ -21416,7 +21416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>139</v>
       </c>
@@ -21568,7 +21568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>140</v>
       </c>
@@ -21720,7 +21720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>141</v>
       </c>
@@ -21872,7 +21872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>142</v>
       </c>
@@ -22024,7 +22024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>143</v>
       </c>
@@ -22176,7 +22176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>144</v>
       </c>
@@ -22328,7 +22328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>145</v>
       </c>
@@ -22480,7 +22480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>146</v>
       </c>
@@ -22632,7 +22632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>147</v>
       </c>
@@ -22784,7 +22784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A147">
         <v>148</v>
       </c>
@@ -22936,7 +22936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A148">
         <v>149</v>
       </c>
@@ -23088,7 +23088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>150</v>
       </c>
@@ -23240,7 +23240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A150">
         <v>151</v>
       </c>
@@ -23392,7 +23392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A151">
         <v>152</v>
       </c>
@@ -23544,7 +23544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A152">
         <v>153</v>
       </c>
@@ -23696,7 +23696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A153">
         <v>154</v>
       </c>
@@ -23848,7 +23848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A154">
         <v>155</v>
       </c>
@@ -24000,7 +24000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A155">
         <v>156</v>
       </c>
@@ -24152,7 +24152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A156">
         <v>157</v>
       </c>
@@ -24304,7 +24304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A157">
         <v>158</v>
       </c>
@@ -24456,7 +24456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A158">
         <v>159</v>
       </c>
@@ -24608,7 +24608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A159">
         <v>160</v>
       </c>
@@ -24760,7 +24760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A160">
         <v>161</v>
       </c>
@@ -24912,7 +24912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A161">
         <v>162</v>
       </c>
@@ -25064,7 +25064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A162">
         <v>163</v>
       </c>
@@ -25216,7 +25216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A163">
         <v>164</v>
       </c>
@@ -25368,7 +25368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A164">
         <v>165</v>
       </c>
@@ -25520,7 +25520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A165">
         <v>166</v>
       </c>
@@ -25672,7 +25672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A166">
         <v>167</v>
       </c>
@@ -25824,7 +25824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A167">
         <v>168</v>
       </c>
@@ -25976,7 +25976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A168">
         <v>169</v>
       </c>
@@ -26128,7 +26128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A169">
         <v>170</v>
       </c>
@@ -26280,7 +26280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A170">
         <v>171</v>
       </c>
@@ -26432,7 +26432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A171">
         <v>172</v>
       </c>
@@ -26584,7 +26584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A172">
         <v>173</v>
       </c>
@@ -26736,7 +26736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A173">
         <v>174</v>
       </c>
@@ -26888,7 +26888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A174">
         <v>175</v>
       </c>
@@ -27040,7 +27040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A175">
         <v>176</v>
       </c>
@@ -27192,7 +27192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A176">
         <v>177</v>
       </c>
@@ -27344,7 +27344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A177">
         <v>178</v>
       </c>
@@ -27496,7 +27496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A178">
         <v>179</v>
       </c>
@@ -27648,7 +27648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A179">
         <v>180</v>
       </c>
@@ -27800,7 +27800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A180">
         <v>181</v>
       </c>
@@ -27952,7 +27952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A181">
         <v>182</v>
       </c>
@@ -28104,7 +28104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A182">
         <v>183</v>
       </c>
@@ -28256,7 +28256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A183">
         <v>184</v>
       </c>
@@ -28408,7 +28408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A184">
         <v>185</v>
       </c>
@@ -28560,7 +28560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A185">
         <v>186</v>
       </c>
@@ -28712,7 +28712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A186">
         <v>187</v>
       </c>
@@ -28864,7 +28864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A187">
         <v>188</v>
       </c>
@@ -29016,7 +29016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A188">
         <v>189</v>
       </c>
@@ -29168,7 +29168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A189">
         <v>190</v>
       </c>
@@ -29320,7 +29320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A190">
         <v>191</v>
       </c>
@@ -29472,7 +29472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A191">
         <v>193</v>
       </c>
@@ -29624,7 +29624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A192">
         <v>194</v>
       </c>
@@ -29776,7 +29776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A193">
         <v>195</v>
       </c>
@@ -29928,7 +29928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A194">
         <v>196</v>
       </c>
@@ -30080,7 +30080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A195">
         <v>197</v>
       </c>
@@ -30232,7 +30232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A196">
         <v>199</v>
       </c>
@@ -30384,7 +30384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A197">
         <v>200</v>
       </c>
@@ -30536,7 +30536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A198">
         <v>201</v>
       </c>
@@ -30688,7 +30688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A199">
         <v>202</v>
       </c>
@@ -30840,7 +30840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A200">
         <v>203</v>
       </c>
@@ -30992,7 +30992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A201">
         <v>204</v>
       </c>
@@ -31144,7 +31144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A202">
         <v>205</v>
       </c>
@@ -31296,7 +31296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A203">
         <v>206</v>
       </c>
@@ -31448,7 +31448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A204">
         <v>207</v>
       </c>
@@ -31600,7 +31600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A205">
         <v>208</v>
       </c>
@@ -31752,7 +31752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A206">
         <v>209</v>
       </c>
@@ -31904,7 +31904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A207">
         <v>210</v>
       </c>
@@ -32056,7 +32056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A208">
         <v>211</v>
       </c>
@@ -32208,7 +32208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A209">
         <v>212</v>
       </c>
@@ -32360,7 +32360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A210">
         <v>213</v>
       </c>
@@ -32512,7 +32512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A211">
         <v>214</v>
       </c>
@@ -32664,7 +32664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A212">
         <v>216</v>
       </c>
@@ -32816,7 +32816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A213">
         <v>217</v>
       </c>
@@ -32968,7 +32968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A214">
         <v>218</v>
       </c>
@@ -33120,7 +33120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A215">
         <v>219</v>
       </c>
@@ -33272,7 +33272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A216">
         <v>220</v>
       </c>
@@ -33424,7 +33424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A217">
         <v>221</v>
       </c>
@@ -33576,7 +33576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A218">
         <v>222</v>
       </c>
@@ -33728,7 +33728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A219">
         <v>223</v>
       </c>
@@ -33880,7 +33880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A220">
         <v>224</v>
       </c>
@@ -34032,7 +34032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A221">
         <v>225</v>
       </c>
@@ -34184,7 +34184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A222">
         <v>226</v>
       </c>
@@ -34336,7 +34336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A223">
         <v>227</v>
       </c>
@@ -34488,7 +34488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A224">
         <v>228</v>
       </c>
@@ -34640,7 +34640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A225">
         <v>229</v>
       </c>
@@ -34792,7 +34792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A226">
         <v>230</v>
       </c>
@@ -34944,7 +34944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A227">
         <v>231</v>
       </c>
@@ -35096,7 +35096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A228">
         <v>232</v>
       </c>
@@ -35203,7 +35203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A229">
         <v>233</v>
       </c>
@@ -35355,7 +35355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:50" x14ac:dyDescent="0.4">
       <c r="A230">
         <v>234</v>
       </c>

</xml_diff>